<commit_message>
remove temporarily images, add services_categories.txt
</commit_message>
<xml_diff>
--- a/biwg_dashboards_2.xlsx
+++ b/biwg_dashboards_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcondeixa/repositories/brazilian_immigrant_women_in_germany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A15BEC6-7D11-C04D-B2CD-C86CCFDB10B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97332B-D9C5-0D41-8A3A-A9C530D8734B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
@@ -31,20 +31,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">offered_services!$A$1:$C$26</definedName>
     <definedName name="_xlchart.v5.0" hidden="1">city!$A$46</definedName>
     <definedName name="_xlchart.v5.1" hidden="1">city!$A$47:$A$59</definedName>
-    <definedName name="_xlchart.v5.10" hidden="1">city!$B$46</definedName>
-    <definedName name="_xlchart.v5.11" hidden="1">city!$B$47:$B$59</definedName>
-    <definedName name="_xlchart.v5.12" hidden="1">city!$A$46</definedName>
-    <definedName name="_xlchart.v5.13" hidden="1">city!$A$47:$A$59</definedName>
-    <definedName name="_xlchart.v5.14" hidden="1">city!$B$46</definedName>
-    <definedName name="_xlchart.v5.15" hidden="1">city!$B$47:$B$59</definedName>
     <definedName name="_xlchart.v5.2" hidden="1">city!$B$46</definedName>
     <definedName name="_xlchart.v5.3" hidden="1">city!$B$47:$B$59</definedName>
     <definedName name="_xlchart.v5.4" hidden="1">city!$A$46</definedName>
     <definedName name="_xlchart.v5.5" hidden="1">city!$A$47:$A$59</definedName>
     <definedName name="_xlchart.v5.6" hidden="1">city!$B$46</definedName>
     <definedName name="_xlchart.v5.7" hidden="1">city!$B$47:$B$59</definedName>
-    <definedName name="_xlchart.v5.8" hidden="1">city!$A$46</definedName>
-    <definedName name="_xlchart.v5.9" hidden="1">city!$A$47:$A$59</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">dashboard1!$N$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -4651,7 +4643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5251518C-499E-194E-93EC-6281AB53B1A4}" type="CELLRANGE">
+                    <a:fld id="{817DE82D-E362-F64D-BB7B-CCBE9B3AD5D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4690,7 +4682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0303D1B9-D023-3C41-B9FB-3F08D6070B0C}" type="CELLRANGE">
+                    <a:fld id="{9F844084-A6A0-A943-981D-5B683B1FCAE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4729,7 +4721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{695B2A2D-8A06-9440-8F38-A8EBA65D8087}" type="CELLRANGE">
+                    <a:fld id="{F80952AE-7350-FD4A-8DBA-AFF7C94DF5D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4768,7 +4760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{621A7195-2961-5E43-A0A9-4787867BB27E}" type="CELLRANGE">
+                    <a:fld id="{57924AEA-DB0C-3844-865C-FE3689E93D48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4807,7 +4799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{576CB61B-76E0-F144-A398-0ACB7AD88CD4}" type="CELLRANGE">
+                    <a:fld id="{6DD0827D-21A4-1F4A-9788-7A1F5AEEBC5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4846,7 +4838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F86041A2-2A2A-514E-9485-46F0821D6A2E}" type="CELLRANGE">
+                    <a:fld id="{48BBB395-7AA4-4F45-8D75-40DFBDBFD3CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4879,7 +4871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7883A928-047B-0E4D-B262-492E0A294C74}" type="CELLRANGE">
+                    <a:fld id="{B16C6A3A-B581-014D-A387-05CC701EC184}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4913,7 +4905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{793D7B87-E9E2-1F4E-BBE0-FD6A482B648B}" type="CELLRANGE">
+                    <a:fld id="{06EE9AEE-C1CA-944E-BD2B-184F2F31BD06}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4947,7 +4939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBF3638E-3056-6048-ADFF-B9AF6823AF38}" type="CELLRANGE">
+                    <a:fld id="{6E7EE925-60EF-5241-AC70-F1760C501634}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4981,7 +4973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D82B2E20-49CA-0C48-AB5C-B509AD8E68BE}" type="CELLRANGE">
+                    <a:fld id="{6135354F-66E6-0140-B8F0-BA066EBE1527}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5015,7 +5007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A888DB4-CA59-EB45-827B-9B5531B3777B}" type="CELLRANGE">
+                    <a:fld id="{BE762CE3-9269-3D40-A162-68395403187B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5049,7 +5041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{707E6326-4451-0546-B7CC-B9E6F9094DA5}" type="CELLRANGE">
+                    <a:fld id="{1ABBD3AA-819A-AA4A-89D0-510E921DED6F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5083,7 +5075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D0BEF9C-B17D-8144-A4B1-AB62BC29CA2D}" type="CELLRANGE">
+                    <a:fld id="{879B1620-7595-7240-9730-5292BAAA0764}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5117,7 +5109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{307C36B0-C15C-E340-8DC7-9DBD734B2B1A}" type="CELLRANGE">
+                    <a:fld id="{45E89895-B465-AA4D-8D35-0B2622094D34}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5151,7 +5143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8FC03A5-DC26-C847-B90B-D25BC0099802}" type="CELLRANGE">
+                    <a:fld id="{39FA82AC-BA0D-3543-8EDE-A3A857E0DF44}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5185,7 +5177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D4760D6-AACD-D24C-B5C3-258D87B22489}" type="CELLRANGE">
+                    <a:fld id="{9A89EEA3-76C5-D945-BBDF-B8992471CEF2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5219,7 +5211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5E01929-9E75-4343-8D32-5DF2650EAAF0}" type="CELLRANGE">
+                    <a:fld id="{4D6E89D9-D357-174C-B00E-3939DC4E69A6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5808,7 +5800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD0CB893-3113-134C-9630-481DB536D27F}" type="CELLRANGE">
+                    <a:fld id="{D123F0A8-3B61-5E44-B0FC-2488FC2AA378}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5906,7 +5898,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{FCD72A81-5AF6-EE4C-B3A4-4CBFB731E64A}" type="CELLRANGE">
+                    <a:fld id="{7A468A63-4776-7C4C-AA67-6761CB5E4381}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -5982,7 +5974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC8AD63B-E6BD-7745-A3B5-F1363CB20748}" type="CELLRANGE">
+                    <a:fld id="{A58B96A8-BFD6-DB41-A74C-4B1E83F9A456}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6016,7 +6008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23850A4D-DA9C-4945-8909-E48DAD6A6C5F}" type="CELLRANGE">
+                    <a:fld id="{A7CF0B14-EF62-1648-A4AE-8156D86AB885}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6056,7 +6048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3B11189-CCA3-BF41-A3AB-1D7E258968B8}" type="CELLRANGE">
+                    <a:fld id="{0D207B61-8089-704B-8781-BF4762D3CB1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6099,7 +6091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{948280A0-EABC-D947-8113-29BCFB621227}" type="CELLRANGE">
+                    <a:fld id="{9BF6CFB3-D461-E04D-8550-497D430D28A0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6139,7 +6131,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B9CE193-B52C-344A-AC5B-BF08F1A62AF1}" type="CELLRANGE">
+                    <a:fld id="{EFF91AEA-E33F-454A-AABE-A07E01C502FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6178,7 +6170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9A34C72-300E-BD43-AEB9-0C0B6D0BD501}" type="CELLRANGE">
+                    <a:fld id="{6266A322-EFA8-3A4C-9177-F9A233D5F9DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6211,7 +6203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{094D1823-ECA6-DE44-B47F-2A23E0B5139C}" type="CELLRANGE">
+                    <a:fld id="{3DE76B4C-F6A8-444C-83B1-24CB3306E272}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9573,7 +9565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45F5FE70-6EAC-2B4F-A63B-123F3FB13897}" type="CELLRANGE">
+                    <a:fld id="{35FCC34B-BFD2-5D4D-B2D8-CC825C9B1118}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9606,7 +9598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EF0FB82-3062-E247-8921-4AEF32E36504}" type="CELLRANGE">
+                    <a:fld id="{51477557-2B09-724C-A026-8724EAF5A7F0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9640,7 +9632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A66238F2-145A-A84E-B075-CC49B6BE2FA2}" type="CELLRANGE">
+                    <a:fld id="{1AB43B40-818B-E74A-9223-56FB7BEFCC48}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9674,7 +9666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC43859A-8654-154A-B11B-89CB799FC9C5}" type="CELLRANGE">
+                    <a:fld id="{856A9647-E57F-3847-8C24-1791FB69E3AB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9708,7 +9700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B14BCB42-9BD0-9E4F-A132-D364EF30E8C0}" type="CELLRANGE">
+                    <a:fld id="{FF6ECCF3-F4F5-FE40-AF19-3751E830C0AB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9742,7 +9734,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2D2E194-CDB4-8244-9B24-E291A2469C2F}" type="CELLRANGE">
+                    <a:fld id="{137D9740-70EC-6D4A-AF7A-03EFDAD18F24}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10913,7 +10905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{209A1D1D-BDB5-DB4B-839F-976789398C69}" type="CELLRANGE">
+                    <a:fld id="{DCAD0CD6-71E2-5740-AC48-168C0B8CACF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10946,7 +10938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC337761-5EB7-2545-BA7C-6B28BB491BFF}" type="CELLRANGE">
+                    <a:fld id="{3B5473BF-307B-4045-8FF1-62ABDD576DD3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10980,7 +10972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70048546-CBC9-8E40-A5B8-C9BC025D8004}" type="CELLRANGE">
+                    <a:fld id="{BA51264A-0C57-3341-BB58-E899C54589DD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11014,7 +11006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D11CB6B8-D921-8A46-AE56-9D056726E6B5}" type="CELLRANGE">
+                    <a:fld id="{BB70B702-DC29-0548-A03A-47D74AC62102}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11048,7 +11040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54F1453E-974C-C24D-976C-105B4723E47D}" type="CELLRANGE">
+                    <a:fld id="{4DF6E23A-3D6D-0D4D-81C3-135F37CBF5F3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11082,7 +11074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37C32BE7-078F-5948-88D7-FBC856DDB79E}" type="CELLRANGE">
+                    <a:fld id="{D2CBC27A-C1CC-084D-91A7-10F37EA14EA4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11116,7 +11108,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB2628EE-0910-9B41-87ED-6B24E6541FD6}" type="CELLRANGE">
+                    <a:fld id="{50C22F03-9A3C-3649-B16A-97319C534DB6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11894,7 +11886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{883B4C32-FB8C-174A-9ABA-6E51D3CE945E}" type="CELLRANGE">
+                    <a:fld id="{04F68BD6-64B6-A242-BB70-9BA3129AA9B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11992,7 +11984,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E76722CB-4645-9A42-BEBE-6DD4E7A7962D}" type="CELLRANGE">
+                    <a:fld id="{0F412D27-636F-0F4D-951C-7B0CF690FCB3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -12068,7 +12060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FCF7E18-DF41-1C4D-8A34-6E4E34F7921D}" type="CELLRANGE">
+                    <a:fld id="{16691AB5-FF03-1242-9027-4BDEFFF8EA8F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12102,7 +12094,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B57CB4C-3D8F-C74E-9B9A-5E7AFC010E7D}" type="CELLRANGE">
+                    <a:fld id="{743FA537-8004-E241-A077-48384C2FB099}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12156,7 +12148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2256173F-9199-DB42-9B00-626990C4BCF4}" type="CELLRANGE">
+                    <a:fld id="{78DC9D85-36BA-E549-9421-87352DC8A89A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12210,7 +12202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99272229-1F74-4A4D-BE24-646F1738B437}" type="CELLRANGE">
+                    <a:fld id="{9ED7A024-06EF-174A-9FD4-F3891B2C762D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13446,7 +13438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88DB5742-16E6-674C-A062-5EB106CB0DBD}" type="CELLRANGE">
+                    <a:fld id="{1C30321F-DC4E-E94C-9BBA-4BD556AADAD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13479,7 +13471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{056FC1B8-D69D-B741-82C9-1760CF313126}" type="CELLRANGE">
+                    <a:fld id="{3FB0F290-64CA-E146-9271-8510E5B08B46}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13513,7 +13505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9696C98B-700E-D247-870E-3F0951B1BD1D}" type="CELLRANGE">
+                    <a:fld id="{C49840AE-0742-444D-8F49-714B84FE1352}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13547,7 +13539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94BFB6B2-0EC5-4D44-8046-61001EB1F52D}" type="CELLRANGE">
+                    <a:fld id="{1C86F20A-3A81-8743-AD88-62C7094B1F91}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13581,7 +13573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED07B56F-17A5-9549-A1B1-20486FC73CA7}" type="CELLRANGE">
+                    <a:fld id="{1D0389E5-2E1D-E84E-80F5-04709B28C0C9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13615,7 +13607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C109F26E-837B-9E46-AA27-7950BB0E3945}" type="CELLRANGE">
+                    <a:fld id="{58ADC152-94BC-E14C-90BC-35994631E399}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -40090,7 +40082,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="13538011" cy="7311453"/>
+          <a:ext cx="13499335" cy="7290298"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="13538011" cy="7311453"/>
         </a:xfrm>
@@ -41391,7 +41383,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>RESTAURANTS : healthy food, Brazilian food, in self-service format, Brazilian weets, rental party rooms</a:t>
+                  <a:t>RESTAURANTS : healthy food, Brazilian food, in self-service format, Brazilian food, rental party rooms</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41447,7 +41439,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>SOCIAL  SERVICES : lawyer, integration activities,  newly arrived, imigration, victims of domestic violence, translation in essential services</a:t>
+                  <a:t>SOCIAL  SERVICES : lawyer, integration activities,  newly arrived, immigration, victims of domestic violence, translation in essential services</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41492,7 +41484,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>MENTAL  HEALTH : psicology, psychiatry, wellness</a:t>
+                  <a:t>MENTAL  HEALTH : psychology, psychiatry, wellness</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41983,20 +41975,6 @@
               <a:p>
                 <a:pPr algn="l"/>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
                       <a:schemeClr val="bg1">
@@ -42008,7 +41986,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>JOB &amp; BUSINESS: digital marketing,corporate communication,advertisement, data analytics, digital marketing, business consulting, ilustrator, photography, career coach, life coach, translation</a:t>
+                  <a:t>JOB &amp; BUSINESS: digital marketing, corporate communication, advertisement, data analytics, digital marketing, business consulting, illustrator, photography, career coach, life coach, translation</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750">
@@ -42066,7 +42044,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>ART &amp; CULTURE: education,exchange programs, dance classes</a:t>
+                  <a:t>ART &amp; CULTURE: education, exchange programs, dance classes</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750">
@@ -42251,7 +42229,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>FOOD : baby food, backery</a:t>
+                  <a:t>FOOD : baby food, bakery</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="750">
                   <a:solidFill>
@@ -43086,50 +43064,6 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>22478</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>157345</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>781781</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>41313</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DBA544-DA28-8271-857D-D08B30AD2C4D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14925310" y="3753805"/>
-          <a:ext cx="7772400" cy="4199720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -47293,7 +47227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26052D2A-800B-3140-B601-B949F26C3F41}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
@@ -48019,8 +47953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
add images, fix duplicated categories in the txt
</commit_message>
<xml_diff>
--- a/biwg_dashboards_2.xlsx
+++ b/biwg_dashboards_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcondeixa/repositories/brazilian_immigrant_women_in_germany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC97332B-D9C5-0D41-8A3A-A9C530D8734B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8997979B-0E91-B54A-B85C-5D00D89851A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4643,7 +4643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{817DE82D-E362-F64D-BB7B-CCBE9B3AD5D0}" type="CELLRANGE">
+                    <a:fld id="{9F7B4510-4B4A-1E47-86F4-918A17439D23}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4682,7 +4682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F844084-A6A0-A943-981D-5B683B1FCAE7}" type="CELLRANGE">
+                    <a:fld id="{AC505009-6488-B643-A958-E93CC13751AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4721,7 +4721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F80952AE-7350-FD4A-8DBA-AFF7C94DF5D0}" type="CELLRANGE">
+                    <a:fld id="{1038BCC5-80DB-1E4D-8128-850095E6918E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4760,7 +4760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57924AEA-DB0C-3844-865C-FE3689E93D48}" type="CELLRANGE">
+                    <a:fld id="{16EEFC6D-AAC3-3C4C-9AB5-230B7F96E5A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4799,7 +4799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DD0827D-21A4-1F4A-9788-7A1F5AEEBC5D}" type="CELLRANGE">
+                    <a:fld id="{639D0E66-F320-4445-B512-6FCF8823AA1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4838,7 +4838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48BBB395-7AA4-4F45-8D75-40DFBDBFD3CA}" type="CELLRANGE">
+                    <a:fld id="{672AE988-1C80-1F46-AE89-A50101B4564A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4871,7 +4871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B16C6A3A-B581-014D-A387-05CC701EC184}" type="CELLRANGE">
+                    <a:fld id="{4CCB907A-AC55-DC43-92C3-D391DF8EF161}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4905,7 +4905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06EE9AEE-C1CA-944E-BD2B-184F2F31BD06}" type="CELLRANGE">
+                    <a:fld id="{7D9518B7-CDD5-514F-B3F2-841C97C78A9F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4939,7 +4939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E7EE925-60EF-5241-AC70-F1760C501634}" type="CELLRANGE">
+                    <a:fld id="{70837633-2DA3-DF4D-9C7D-ECF67A546B05}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4973,7 +4973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6135354F-66E6-0140-B8F0-BA066EBE1527}" type="CELLRANGE">
+                    <a:fld id="{7BB3599F-E5F9-CA49-9AAE-990EF5876C73}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5007,7 +5007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE762CE3-9269-3D40-A162-68395403187B}" type="CELLRANGE">
+                    <a:fld id="{9629DEDD-F68C-3E44-90C5-37CB6D0F0B93}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5041,7 +5041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1ABBD3AA-819A-AA4A-89D0-510E921DED6F}" type="CELLRANGE">
+                    <a:fld id="{01A3C04F-0ECF-1F49-BEEC-94A0999B5B8F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5075,7 +5075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{879B1620-7595-7240-9730-5292BAAA0764}" type="CELLRANGE">
+                    <a:fld id="{0AEEF5B0-6D55-6643-A0A0-88D6411B8E28}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5109,7 +5109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45E89895-B465-AA4D-8D35-0B2622094D34}" type="CELLRANGE">
+                    <a:fld id="{95EA5491-7757-9244-9BF2-E2B3B970F9E0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5143,7 +5143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39FA82AC-BA0D-3543-8EDE-A3A857E0DF44}" type="CELLRANGE">
+                    <a:fld id="{88B26FC1-9EDC-AC49-B3A7-E79495AC31EB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5177,7 +5177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A89EEA3-76C5-D945-BBDF-B8992471CEF2}" type="CELLRANGE">
+                    <a:fld id="{CFAE4D59-C096-3D4D-B674-7C434C55CC79}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5211,7 +5211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D6E89D9-D357-174C-B00E-3939DC4E69A6}" type="CELLRANGE">
+                    <a:fld id="{565A11A0-1418-BC47-B475-1FD858059AC3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5800,7 +5800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D123F0A8-3B61-5E44-B0FC-2488FC2AA378}" type="CELLRANGE">
+                    <a:fld id="{C1FB8337-DCF9-8847-91EC-CAE64DEC1748}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5898,7 +5898,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7A468A63-4776-7C4C-AA67-6761CB5E4381}" type="CELLRANGE">
+                    <a:fld id="{E2114000-94AE-A544-BA21-3555D00B4976}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -5974,7 +5974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A58B96A8-BFD6-DB41-A74C-4B1E83F9A456}" type="CELLRANGE">
+                    <a:fld id="{B28529D5-7E7A-824E-9EEC-9A782F10F5F2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6008,7 +6008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7CF0B14-EF62-1648-A4AE-8156D86AB885}" type="CELLRANGE">
+                    <a:fld id="{A6F6C44B-DEFF-7743-A9EA-BA1D31D94D20}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6048,7 +6048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D207B61-8089-704B-8781-BF4762D3CB1C}" type="CELLRANGE">
+                    <a:fld id="{A7944F21-00FF-2C4B-B341-766BC0C044D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6091,7 +6091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BF6CFB3-D461-E04D-8550-497D430D28A0}" type="CELLRANGE">
+                    <a:fld id="{C6982735-EBB0-9B43-962F-C1CA2A156233}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6131,7 +6131,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFF91AEA-E33F-454A-AABE-A07E01C502FF}" type="CELLRANGE">
+                    <a:fld id="{48E4CA5A-259F-F940-BA57-0C9BF34FE6B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6170,7 +6170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6266A322-EFA8-3A4C-9177-F9A233D5F9DC}" type="CELLRANGE">
+                    <a:fld id="{ADAC0407-133D-0144-BD39-A9205BCDF5D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6203,7 +6203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DE76B4C-F6A8-444C-83B1-24CB3306E272}" type="CELLRANGE">
+                    <a:fld id="{EA54CCD9-F277-7B42-98B5-42A489B62645}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9565,7 +9565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35FCC34B-BFD2-5D4D-B2D8-CC825C9B1118}" type="CELLRANGE">
+                    <a:fld id="{90E8F6D4-D5D1-0A4A-8CF1-21DB039F4829}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9598,7 +9598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51477557-2B09-724C-A026-8724EAF5A7F0}" type="CELLRANGE">
+                    <a:fld id="{4EA25ED8-C25E-2341-8FAF-4FEA6E097E65}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9632,7 +9632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1AB43B40-818B-E74A-9223-56FB7BEFCC48}" type="CELLRANGE">
+                    <a:fld id="{E6363514-6263-4F49-991F-3E35E4EDE760}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9666,7 +9666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{856A9647-E57F-3847-8C24-1791FB69E3AB}" type="CELLRANGE">
+                    <a:fld id="{4771AE34-3F62-DC49-ACC8-79E44D4FAD0D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9700,7 +9700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF6ECCF3-F4F5-FE40-AF19-3751E830C0AB}" type="CELLRANGE">
+                    <a:fld id="{331C3DFC-F295-484F-9CA7-A2FC96144AEA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9734,7 +9734,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{137D9740-70EC-6D4A-AF7A-03EFDAD18F24}" type="CELLRANGE">
+                    <a:fld id="{C0B60EEC-2EC2-DE4A-9993-A1C900578C5F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10905,7 +10905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCAD0CD6-71E2-5740-AC48-168C0B8CACF6}" type="CELLRANGE">
+                    <a:fld id="{9B8F5466-3F48-C345-8512-77509DDE4BCE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10938,7 +10938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B5473BF-307B-4045-8FF1-62ABDD576DD3}" type="CELLRANGE">
+                    <a:fld id="{FA2F9414-7094-1745-A5FF-D8ABE94B4A0A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10972,7 +10972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA51264A-0C57-3341-BB58-E899C54589DD}" type="CELLRANGE">
+                    <a:fld id="{94F9C2F0-B457-C542-8DB7-02C146DAAF1A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11006,7 +11006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB70B702-DC29-0548-A03A-47D74AC62102}" type="CELLRANGE">
+                    <a:fld id="{D4CE1579-699D-EE40-81E3-F43233A576E8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11040,7 +11040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DF6E23A-3D6D-0D4D-81C3-135F37CBF5F3}" type="CELLRANGE">
+                    <a:fld id="{E9005817-98BA-D446-A2F7-E34BB8AF5B1D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11074,7 +11074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2CBC27A-C1CC-084D-91A7-10F37EA14EA4}" type="CELLRANGE">
+                    <a:fld id="{6D3D9AE1-5481-914E-9E2E-5FAAD371A9C6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11108,7 +11108,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50C22F03-9A3C-3649-B16A-97319C534DB6}" type="CELLRANGE">
+                    <a:fld id="{CC281047-6D6E-FD4C-AC52-5BB0745AA8D7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11886,7 +11886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04F68BD6-64B6-A242-BB70-9BA3129AA9B4}" type="CELLRANGE">
+                    <a:fld id="{2356F329-B5B7-1247-915A-148E899A00B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11984,7 +11984,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{0F412D27-636F-0F4D-951C-7B0CF690FCB3}" type="CELLRANGE">
+                    <a:fld id="{E30B9DD2-3AA0-054E-AA7D-7F32AF87B6F0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -12060,7 +12060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16691AB5-FF03-1242-9027-4BDEFFF8EA8F}" type="CELLRANGE">
+                    <a:fld id="{8BAD9CE4-7FC2-D54C-A013-D473AE074D5F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12094,7 +12094,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{743FA537-8004-E241-A077-48384C2FB099}" type="CELLRANGE">
+                    <a:fld id="{F7AB603C-8B6F-3940-B9E1-43858A8EF9A2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12148,7 +12148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78DC9D85-36BA-E549-9421-87352DC8A89A}" type="CELLRANGE">
+                    <a:fld id="{FA0714AF-3E7F-B24F-B5AE-6D5F184E6EF1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12202,7 +12202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ED7A024-06EF-174A-9FD4-F3891B2C762D}" type="CELLRANGE">
+                    <a:fld id="{1D482B6F-0FED-6345-B0E2-CB7A2313003F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13438,7 +13438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C30321F-DC4E-E94C-9BBA-4BD556AADAD0}" type="CELLRANGE">
+                    <a:fld id="{75B0A94D-AFB5-5E42-9471-EFECC2ED5BB3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13471,7 +13471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FB0F290-64CA-E146-9271-8510E5B08B46}" type="CELLRANGE">
+                    <a:fld id="{DBEF6864-0356-D24E-B6FC-936EE50BB770}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13505,7 +13505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C49840AE-0742-444D-8F49-714B84FE1352}" type="CELLRANGE">
+                    <a:fld id="{460BAADF-DBC2-9E4E-AB87-2824EF9A1939}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13539,7 +13539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C86F20A-3A81-8743-AD88-62C7094B1F91}" type="CELLRANGE">
+                    <a:fld id="{BAAF5676-2704-9C4D-A66E-6E9EF244D0C4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13573,7 +13573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D0389E5-2E1D-E84E-80F5-04709B28C0C9}" type="CELLRANGE">
+                    <a:fld id="{E594288A-35CE-7F43-B9D0-3170ABC73360}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13607,7 +13607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58ADC152-94BC-E14C-90BC-35994631E399}" type="CELLRANGE">
+                    <a:fld id="{F1819347-8FFA-8344-8723-891BE0C930AB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -39709,166 +39709,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>68258</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>170551</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>276656</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>168269</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000014000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1712862" y="7635227"/>
-          <a:ext cx="208398" cy="171315"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>380546</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>35677</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>560200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>36097</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000017000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:alphaModFix amt="97000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2025150" y="7673950"/>
-          <a:ext cx="179654" cy="174018"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>602699</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>163731</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>465731</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>154872</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000018000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:duotone>
-            <a:prstClr val="black"/>
-            <a:srgbClr val="D9C3A5">
-              <a:tint val="50000"/>
-              <a:satMod val="180000"/>
-            </a:srgbClr>
-          </a:duotone>
-          <a:alphaModFix/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2247303" y="7628407"/>
-          <a:ext cx="685334" cy="164738"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>379106</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -39899,7 +39739,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -40049,7 +39889,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -40120,7 +39960,7 @@
             </xdr:cNvPicPr>
           </xdr:nvPicPr>
           <xdr:blipFill rotWithShape="1">
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
               <a:extLst>
                 <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                   <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -41151,7 +40991,7 @@
             </xdr:xfrm>
             <a:graphic>
               <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-                <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+                <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
               </a:graphicData>
             </a:graphic>
           </xdr:graphicFrame>
@@ -41624,34 +41464,6 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>JOB &amp; BUSINESS : professional outplacement, support for entrepreneurship</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
                   <a:t>DELIVERY : pharmacy, Brazilian food, furniture assembly and transportation</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41818,8 +41630,43 @@
                     <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
+                  <a:t> , </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>education, exchange programs, dance classes</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> </a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
               <a:p>
                 <a:endParaRPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41973,7 +41820,23 @@
                 </a:r>
               </a:p>
               <a:p>
-                <a:pPr algn="l"/>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
                     <a:solidFill>
@@ -41986,7 +41849,35 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>JOB &amp; BUSINESS: digital marketing, corporate communication, advertisement, data analytics, digital marketing, business consulting, illustrator, photography, career coach, life coach, translation</a:t>
+                  <a:t>JOB &amp; BUSINESS: </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>professional outplacement, support for entrepreneurship,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> digital marketing, corporate communication, advertisement, data analytics, digital marketing, business consulting, illustrator, photography, career coach, life coach, translation</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750">
@@ -42016,35 +41907,6 @@
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
                   <a:t>HOME SERVICES: tidying up</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>ART &amp; CULTURE: education, exchange programs, dance classes</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750">
@@ -47954,7 +47816,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+      <selection activeCell="L45" sqref="L45:L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
add line break in txt, update dashboards add image for preview
</commit_message>
<xml_diff>
--- a/biwg_dashboards_2.xlsx
+++ b/biwg_dashboards_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcondeixa/repositories/brazilian_immigrant_women_in_germany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8997979B-0E91-B54A-B85C-5D00D89851A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D7D3B-1729-6048-B60A-AA8FAF99C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4643,7 +4643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F7B4510-4B4A-1E47-86F4-918A17439D23}" type="CELLRANGE">
+                    <a:fld id="{9EBDCDDB-FDA4-BE42-882A-2DDD2C56B750}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4682,7 +4682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC505009-6488-B643-A958-E93CC13751AB}" type="CELLRANGE">
+                    <a:fld id="{D2DEFB84-9176-EA4F-B136-3DF608483234}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4721,7 +4721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1038BCC5-80DB-1E4D-8128-850095E6918E}" type="CELLRANGE">
+                    <a:fld id="{803618AF-92FB-0742-9DD2-85F1B589DECD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4760,7 +4760,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16EEFC6D-AAC3-3C4C-9AB5-230B7F96E5A3}" type="CELLRANGE">
+                    <a:fld id="{612B60D2-00E4-9448-9C41-0C3533A58E1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4799,7 +4799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{639D0E66-F320-4445-B512-6FCF8823AA1F}" type="CELLRANGE">
+                    <a:fld id="{6BAC051D-5472-2E4D-96AC-26EB265FAEAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4838,7 +4838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{672AE988-1C80-1F46-AE89-A50101B4564A}" type="CELLRANGE">
+                    <a:fld id="{A58916DD-82CB-AC48-9E11-32D6C9ADD406}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4871,7 +4871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CCB907A-AC55-DC43-92C3-D391DF8EF161}" type="CELLRANGE">
+                    <a:fld id="{89D3DF22-469D-5246-A47C-77F22947C9A1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4905,7 +4905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D9518B7-CDD5-514F-B3F2-841C97C78A9F}" type="CELLRANGE">
+                    <a:fld id="{D8989607-C65A-5F49-B4B0-7CDC8D6398DA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4939,7 +4939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70837633-2DA3-DF4D-9C7D-ECF67A546B05}" type="CELLRANGE">
+                    <a:fld id="{A2BD23D1-B0A9-9A44-B50E-EBC0D2030A78}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4973,7 +4973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BB3599F-E5F9-CA49-9AAE-990EF5876C73}" type="CELLRANGE">
+                    <a:fld id="{BD1BB4E2-1234-A746-B745-D240EC9E14C4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5007,7 +5007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9629DEDD-F68C-3E44-90C5-37CB6D0F0B93}" type="CELLRANGE">
+                    <a:fld id="{ADA2F068-F36B-A247-9667-C37E6B6BC46B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5041,7 +5041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{01A3C04F-0ECF-1F49-BEEC-94A0999B5B8F}" type="CELLRANGE">
+                    <a:fld id="{55C3EFEE-DE86-BC4E-93E7-CA1F9DEE32B2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5075,7 +5075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AEEF5B0-6D55-6643-A0A0-88D6411B8E28}" type="CELLRANGE">
+                    <a:fld id="{C8CF5FE5-F15E-CF42-9BA6-B4EECD410FB8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5109,7 +5109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95EA5491-7757-9244-9BF2-E2B3B970F9E0}" type="CELLRANGE">
+                    <a:fld id="{1F8B645A-8837-8C49-8CEF-0BBCBF24A708}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5143,7 +5143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88B26FC1-9EDC-AC49-B3A7-E79495AC31EB}" type="CELLRANGE">
+                    <a:fld id="{AF93DE46-0465-E24B-8F0E-86FC7573A8ED}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5177,7 +5177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFAE4D59-C096-3D4D-B674-7C434C55CC79}" type="CELLRANGE">
+                    <a:fld id="{FD3805DD-6399-0142-A790-9CA868E035A0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5211,7 +5211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{565A11A0-1418-BC47-B475-1FD858059AC3}" type="CELLRANGE">
+                    <a:fld id="{43738E41-B87B-D148-99B4-F089CE801902}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5800,7 +5800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1FB8337-DCF9-8847-91EC-CAE64DEC1748}" type="CELLRANGE">
+                    <a:fld id="{A589E171-DA1C-1C47-ACA0-0CA0696028C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5898,7 +5898,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E2114000-94AE-A544-BA21-3555D00B4976}" type="CELLRANGE">
+                    <a:fld id="{53D5DD98-0FBA-834C-8F89-21D683EBC552}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -5974,7 +5974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B28529D5-7E7A-824E-9EEC-9A782F10F5F2}" type="CELLRANGE">
+                    <a:fld id="{C32FDFC3-0B20-9E4C-BBFC-28F40919E133}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6008,7 +6008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6F6C44B-DEFF-7743-A9EA-BA1D31D94D20}" type="CELLRANGE">
+                    <a:fld id="{F043A3EC-5A96-F242-B45C-FB61A9C82C97}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6048,7 +6048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7944F21-00FF-2C4B-B341-766BC0C044D2}" type="CELLRANGE">
+                    <a:fld id="{3391BD4E-A14B-7B49-A349-FC126AAC4893}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6091,7 +6091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6982735-EBB0-9B43-962F-C1CA2A156233}" type="CELLRANGE">
+                    <a:fld id="{4E9310C3-F419-F049-93BA-73DF05E8FCB2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6131,7 +6131,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48E4CA5A-259F-F940-BA57-0C9BF34FE6B4}" type="CELLRANGE">
+                    <a:fld id="{E6908668-48EA-1147-8E2D-3A56FE7A07B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6170,7 +6170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADAC0407-133D-0144-BD39-A9205BCDF5D3}" type="CELLRANGE">
+                    <a:fld id="{1A3824D0-DE59-C044-A25C-C1CE4061C64E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6203,7 +6203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA54CCD9-F277-7B42-98B5-42A489B62645}" type="CELLRANGE">
+                    <a:fld id="{81C3D222-477B-DB4D-9A00-4323B1EDCF0E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9565,7 +9565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90E8F6D4-D5D1-0A4A-8CF1-21DB039F4829}" type="CELLRANGE">
+                    <a:fld id="{772220F3-47A6-234C-B5E9-C06524EF42D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9598,7 +9598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EA25ED8-C25E-2341-8FAF-4FEA6E097E65}" type="CELLRANGE">
+                    <a:fld id="{4FB65CD6-6A75-814E-AEE7-8541EC0E4095}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9632,7 +9632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6363514-6263-4F49-991F-3E35E4EDE760}" type="CELLRANGE">
+                    <a:fld id="{A90A14DF-CBF0-2F4E-8A56-CC0365024CDB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9666,7 +9666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4771AE34-3F62-DC49-ACC8-79E44D4FAD0D}" type="CELLRANGE">
+                    <a:fld id="{5B92C167-AD08-464A-B243-7134678D250D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9700,7 +9700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{331C3DFC-F295-484F-9CA7-A2FC96144AEA}" type="CELLRANGE">
+                    <a:fld id="{CC122E3C-80DD-DF47-98E6-1004614FA1E0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9734,7 +9734,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0B60EEC-2EC2-DE4A-9993-A1C900578C5F}" type="CELLRANGE">
+                    <a:fld id="{E93111D0-A0CA-9E42-B9B4-4219A6130EE1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10905,7 +10905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B8F5466-3F48-C345-8512-77509DDE4BCE}" type="CELLRANGE">
+                    <a:fld id="{D508A560-7954-574B-A78F-CBEF5B4F8CA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10938,7 +10938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA2F9414-7094-1745-A5FF-D8ABE94B4A0A}" type="CELLRANGE">
+                    <a:fld id="{8C423794-20F2-3B44-BE76-7134AB15D19D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10972,7 +10972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94F9C2F0-B457-C542-8DB7-02C146DAAF1A}" type="CELLRANGE">
+                    <a:fld id="{09CAC8FA-37F7-BA46-87EB-03DE60571737}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11006,7 +11006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4CE1579-699D-EE40-81E3-F43233A576E8}" type="CELLRANGE">
+                    <a:fld id="{E7C829B7-5E03-F640-AC5F-4DF0921AEA81}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11040,7 +11040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9005817-98BA-D446-A2F7-E34BB8AF5B1D}" type="CELLRANGE">
+                    <a:fld id="{286271BE-11D3-D74B-8BB0-ABA514EE7D85}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11074,7 +11074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D3D9AE1-5481-914E-9E2E-5FAAD371A9C6}" type="CELLRANGE">
+                    <a:fld id="{CB4E9284-8473-DC42-9D69-83457042B96B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11108,7 +11108,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC281047-6D6E-FD4C-AC52-5BB0745AA8D7}" type="CELLRANGE">
+                    <a:fld id="{2332229A-E2CF-3D48-8493-53C912E713EF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11886,7 +11886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2356F329-B5B7-1247-915A-148E899A00B2}" type="CELLRANGE">
+                    <a:fld id="{D9C37EB5-D969-BC4A-8984-1C5FE9530F94}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11984,7 +11984,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E30B9DD2-3AA0-054E-AA7D-7F32AF87B6F0}" type="CELLRANGE">
+                    <a:fld id="{03380A12-19D9-9842-91F7-A00598471539}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -12060,7 +12060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BAD9CE4-7FC2-D54C-A013-D473AE074D5F}" type="CELLRANGE">
+                    <a:fld id="{292B2002-8560-4341-8C9C-133CD29B8B29}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12094,7 +12094,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7AB603C-8B6F-3940-B9E1-43858A8EF9A2}" type="CELLRANGE">
+                    <a:fld id="{C23A691B-1A9D-1645-9EBA-ECFA56BE85B8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12148,7 +12148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA0714AF-3E7F-B24F-B5AE-6D5F184E6EF1}" type="CELLRANGE">
+                    <a:fld id="{70D70B72-96EC-2844-813A-2DC04473626F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12202,7 +12202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D482B6F-0FED-6345-B0E2-CB7A2313003F}" type="CELLRANGE">
+                    <a:fld id="{F67FF1C6-2450-394F-BE65-582379ECF777}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13438,7 +13438,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75B0A94D-AFB5-5E42-9471-EFECC2ED5BB3}" type="CELLRANGE">
+                    <a:fld id="{362B84BE-F02D-7E46-8C0E-14F8D4E74E2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13471,7 +13471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBEF6864-0356-D24E-B6FC-936EE50BB770}" type="CELLRANGE">
+                    <a:fld id="{9D2CBF09-DEE6-CB40-8866-65576A04F03F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13505,7 +13505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{460BAADF-DBC2-9E4E-AB87-2824EF9A1939}" type="CELLRANGE">
+                    <a:fld id="{2C14DE79-EE7F-2042-B0C2-8A564ECA0EF9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13539,7 +13539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAAF5676-2704-9C4D-A66E-6E9EF244D0C4}" type="CELLRANGE">
+                    <a:fld id="{3D8B5DFD-AE69-3A41-8A17-A65D2B79BA75}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13573,7 +13573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E594288A-35CE-7F43-B9D0-3170ABC73360}" type="CELLRANGE">
+                    <a:fld id="{73F6317B-DDE4-0C4E-8BFB-DD5011280872}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13607,7 +13607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1819347-8FFA-8344-8723-891BE0C930AB}" type="CELLRANGE">
+                    <a:fld id="{A873DA69-5C83-184C-A948-08D5F7DADC50}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -42928,6 +42928,50 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>74706</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>643217</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>58270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{949460C0-1D1E-D1F0-1A2F-E5BF227CFF4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3750235" y="8142941"/>
+          <a:ext cx="13500100" cy="7289800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -47812,11 +47856,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45:L46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I46" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -48835,6 +48879,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update excel, removing duplicates and adding ratios in the texts and remove images temporarily
</commit_message>
<xml_diff>
--- a/biwg_dashboards_2.xlsx
+++ b/biwg_dashboards_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcondeixa/repositories/brazilian_immigrant_women_in_germany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D7D3B-1729-6048-B60A-AA8FAF99C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C3B7C8-D96E-1245-B0E4-606997E540E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
@@ -4871,7 +4871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89D3DF22-469D-5246-A47C-77F22947C9A1}" type="CELLRANGE">
+                    <a:fld id="{031EC95E-2554-3C4E-8ADE-69A7FE6D50A7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4905,7 +4905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8989607-C65A-5F49-B4B0-7CDC8D6398DA}" type="CELLRANGE">
+                    <a:fld id="{022F10FB-C2FB-C249-8683-BE958BB2EB5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4939,7 +4939,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2BD23D1-B0A9-9A44-B50E-EBC0D2030A78}" type="CELLRANGE">
+                    <a:fld id="{EA416201-0326-1F40-B061-2BB40FE44863}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4973,7 +4973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD1BB4E2-1234-A746-B745-D240EC9E14C4}" type="CELLRANGE">
+                    <a:fld id="{FDB6B47E-55CB-DC43-ABA2-6FCAB1818937}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5007,7 +5007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADA2F068-F36B-A247-9667-C37E6B6BC46B}" type="CELLRANGE">
+                    <a:fld id="{DF20FBF9-0627-5B4C-87BA-1E13C1A18531}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5041,7 +5041,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55C3EFEE-DE86-BC4E-93E7-CA1F9DEE32B2}" type="CELLRANGE">
+                    <a:fld id="{8030DB35-D614-C04A-A8B9-18B246B67B30}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5075,7 +5075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8CF5FE5-F15E-CF42-9BA6-B4EECD410FB8}" type="CELLRANGE">
+                    <a:fld id="{592BA5BC-BC48-E649-9BB4-DD34C0459305}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5109,7 +5109,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F8B645A-8837-8C49-8CEF-0BBCBF24A708}" type="CELLRANGE">
+                    <a:fld id="{0DE77F5A-8972-DC44-9215-167B6F6F479E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5143,7 +5143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF93DE46-0465-E24B-8F0E-86FC7573A8ED}" type="CELLRANGE">
+                    <a:fld id="{8657AEE2-1DE1-9B46-857F-46BBDBFCF0D2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5177,7 +5177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD3805DD-6399-0142-A790-9CA868E035A0}" type="CELLRANGE">
+                    <a:fld id="{97FFCD5C-03E5-A547-82F3-E39F8B2338CD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5211,7 +5211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43738E41-B87B-D148-99B4-F089CE801902}" type="CELLRANGE">
+                    <a:fld id="{7E0ABB82-503D-8341-AF53-5BF9D7DDF039}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5898,7 +5898,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{53D5DD98-0FBA-834C-8F89-21D683EBC552}" type="CELLRANGE">
+                    <a:fld id="{11C5CBBD-6F17-D64E-95CC-3CECA3B78A5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -5974,7 +5974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C32FDFC3-0B20-9E4C-BBFC-28F40919E133}" type="CELLRANGE">
+                    <a:fld id="{00E70CE0-453E-214E-8C88-2D798A4F4275}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6008,7 +6008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F043A3EC-5A96-F242-B45C-FB61A9C82C97}" type="CELLRANGE">
+                    <a:fld id="{75731E98-DDFD-D84C-8A4C-221727864200}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6091,7 +6091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E9310C3-F419-F049-93BA-73DF05E8FCB2}" type="CELLRANGE">
+                    <a:fld id="{0A0E87DA-BD81-1844-AFD3-37F801EF2A93}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6203,7 +6203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{81C3D222-477B-DB4D-9A00-4323B1EDCF0E}" type="CELLRANGE">
+                    <a:fld id="{17BBB576-2A49-C649-8F49-3F1B23FA9D4E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9565,7 +9565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{772220F3-47A6-234C-B5E9-C06524EF42D9}" type="CELLRANGE">
+                    <a:fld id="{2148BF84-300C-2C4B-8C4E-9084CDC3F954}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9598,7 +9598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FB65CD6-6A75-814E-AEE7-8541EC0E4095}" type="CELLRANGE">
+                    <a:fld id="{D44E3140-B4AE-D344-B2E0-07A192344CE4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9632,7 +9632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A90A14DF-CBF0-2F4E-8A56-CC0365024CDB}" type="CELLRANGE">
+                    <a:fld id="{AA7B32EF-CC54-CD42-B222-2F464845F78E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9666,7 +9666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B92C167-AD08-464A-B243-7134678D250D}" type="CELLRANGE">
+                    <a:fld id="{F14FD23C-79BB-3B40-A7A1-4DC9D3D50A1A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9700,7 +9700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC122E3C-80DD-DF47-98E6-1004614FA1E0}" type="CELLRANGE">
+                    <a:fld id="{87547110-5426-564F-9DB5-EF3C837402BD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9734,7 +9734,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E93111D0-A0CA-9E42-B9B4-4219A6130EE1}" type="CELLRANGE">
+                    <a:fld id="{F3FF54DD-34F1-2842-B63E-FCCD5DCBB4A1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10905,7 +10905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D508A560-7954-574B-A78F-CBEF5B4F8CA6}" type="CELLRANGE">
+                    <a:fld id="{487D8D02-3AAB-D44C-9B11-74B4FBB5E55F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10938,7 +10938,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C423794-20F2-3B44-BE76-7134AB15D19D}" type="CELLRANGE">
+                    <a:fld id="{9F8A3E1D-C1C1-9345-933A-0782D37C2448}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10972,7 +10972,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09CAC8FA-37F7-BA46-87EB-03DE60571737}" type="CELLRANGE">
+                    <a:fld id="{2BD1BD26-C614-9D41-8E06-19CBE07FE030}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11006,7 +11006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7C829B7-5E03-F640-AC5F-4DF0921AEA81}" type="CELLRANGE">
+                    <a:fld id="{29FDF726-34F1-8B4D-B61B-2C2EF4399D47}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11040,7 +11040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{286271BE-11D3-D74B-8BB0-ABA514EE7D85}" type="CELLRANGE">
+                    <a:fld id="{53599692-5244-C744-8177-DD20C685EFA8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11074,7 +11074,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB4E9284-8473-DC42-9D69-83457042B96B}" type="CELLRANGE">
+                    <a:fld id="{B92871D2-AC16-3946-B560-C9A9AC1A33A0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11108,7 +11108,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2332229A-E2CF-3D48-8493-53C912E713EF}" type="CELLRANGE">
+                    <a:fld id="{C7EB9FF5-668C-4C44-A420-63807B9C56AD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11886,7 +11886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D9C37EB5-D969-BC4A-8984-1C5FE9530F94}" type="CELLRANGE">
+                    <a:fld id="{DD4692A3-60CE-FA49-8FAE-7D89611CCBEE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11984,7 +11984,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{03380A12-19D9-9842-91F7-A00598471539}" type="CELLRANGE">
+                    <a:fld id="{601F74A1-0345-0E44-9EB1-B1B70017F969}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -12060,7 +12060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{292B2002-8560-4341-8C9C-133CD29B8B29}" type="CELLRANGE">
+                    <a:fld id="{11AE9168-0AE7-8544-BE62-0A1DD4D731F9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12094,7 +12094,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C23A691B-1A9D-1645-9EBA-ECFA56BE85B8}" type="CELLRANGE">
+                    <a:fld id="{E260127E-ECF0-1E48-A44D-E2B9C6A4E74D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12148,7 +12148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70D70B72-96EC-2844-813A-2DC04473626F}" type="CELLRANGE">
+                    <a:fld id="{8F947103-80CE-0845-BBA3-A87FE0EF08B3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12202,7 +12202,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F67FF1C6-2450-394F-BE65-582379ECF777}" type="CELLRANGE">
+                    <a:fld id="{BEF4B54D-A579-144C-AFCA-1FB7A5B26BE2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13471,7 +13471,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D2CBF09-DEE6-CB40-8866-65576A04F03F}" type="CELLRANGE">
+                    <a:fld id="{E64423F4-00B8-2B43-A35C-319D23D88C15}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13505,7 +13505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C14DE79-EE7F-2042-B0C2-8A564ECA0EF9}" type="CELLRANGE">
+                    <a:fld id="{A725E648-39BE-6C45-A444-1A69A5EA69FD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13539,7 +13539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D8B5DFD-AE69-3A41-8A17-A65D2B79BA75}" type="CELLRANGE">
+                    <a:fld id="{11651ACD-BB43-2343-AFE7-0B997427315B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13573,7 +13573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73F6317B-DDE4-0C4E-8BFB-DD5011280872}" type="CELLRANGE">
+                    <a:fld id="{3C91F424-6181-E84D-8E8D-0CF0023B5CBE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13607,7 +13607,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A873DA69-5C83-184C-A948-08D5F7DADC50}" type="CELLRANGE">
+                    <a:fld id="{0039C79E-1A3D-D049-915B-89D7BFF8632E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -36353,7 +36353,27 @@
                         <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                         <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                       </a:rPr>
-                      <a:t>Most of these women</a:t>
+                      <a:t>An incidence</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="900" spc="110" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="0070C0"/>
+                        </a:solidFill>
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t> of 56%</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="900" spc="110">
+                        <a:solidFill>
+                          <a:srgbClr val="0070C0"/>
+                        </a:solidFill>
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t> of these women</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-GB" sz="900" spc="110" baseline="0">
@@ -36896,10 +36916,10 @@
               </xdr:nvGrpSpPr>
               <xdr:grpSpPr>
                 <a:xfrm>
-                  <a:off x="7223019" y="755748"/>
-                  <a:ext cx="3945713" cy="2968002"/>
+                  <a:off x="7223018" y="755748"/>
+                  <a:ext cx="3894178" cy="2968002"/>
                   <a:chOff x="8021705" y="654260"/>
-                  <a:chExt cx="3932568" cy="3031184"/>
+                  <a:chExt cx="3881205" cy="3031184"/>
                 </a:xfrm>
                 <a:grpFill/>
               </xdr:grpSpPr>
@@ -37111,8 +37131,8 @@
                   </xdr:cNvGraphicFramePr>
                 </xdr:nvGraphicFramePr>
                 <xdr:xfrm>
-                  <a:off x="9817378" y="1030935"/>
-                  <a:ext cx="2136895" cy="1126173"/>
+                  <a:off x="9817378" y="1132874"/>
+                  <a:ext cx="1974968" cy="1024234"/>
                 </xdr:xfrm>
                 <a:graphic>
                   <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -37134,8 +37154,8 @@
                   </xdr:cNvGraphicFramePr>
                 </xdr:nvGraphicFramePr>
                 <xdr:xfrm>
-                  <a:off x="8279239" y="1723555"/>
-                  <a:ext cx="3223809" cy="1738992"/>
+                  <a:off x="8279239" y="1770859"/>
+                  <a:ext cx="3223809" cy="1691688"/>
                 </xdr:xfrm>
                 <a:graphic>
                   <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -37795,7 +37815,7 @@
                           <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                           <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                         </a:rPr>
-                        <a:t>Most</a:t>
+                        <a:t>A ratio of 62%</a:t>
                       </a:r>
                       <a:r>
                         <a:rPr lang="en-GB" sz="1000" spc="110" baseline="0">
@@ -38142,7 +38162,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                       </a:rPr>
-                      <a:t>elementary </a:t>
+                      <a:t>elementary (25%) </a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-GB" sz="900" b="0" i="0" spc="110" baseline="0">
@@ -38178,7 +38198,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                       </a:rPr>
-                      <a:t>basic</a:t>
+                      <a:t>basic (32%)</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-GB" sz="900" b="0" i="0" spc="110" baseline="0">
@@ -39033,7 +39053,7 @@
                 <xdr:spPr>
                   <a:xfrm>
                     <a:off x="414543" y="4146961"/>
-                    <a:ext cx="1630795" cy="851427"/>
+                    <a:ext cx="1533045" cy="851427"/>
                   </a:xfrm>
                   <a:prstGeom prst="roundRect">
                     <a:avLst/>
@@ -39088,7 +39108,7 @@
                         <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                         <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                       </a:rPr>
-                      <a:t>The majority of these women are recent arrivals.</a:t>
+                      <a:t>A fraction of 43% of these women are recent arrivals.</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-GB" sz="1100" b="0">
                       <a:solidFill>
@@ -39468,50 +39488,6 @@
         </xdr:sp>
       </xdr:grpSp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>496047</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>94671</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13401" name="Picture 13400">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5204E43-0DC2-CD26-CCAE-A7AB4D0F808C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="8606118"/>
-          <a:ext cx="7772400" cy="4397729"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -40312,7 +40288,7 @@
                     <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>A rate of 38%  </a:t>
+                  <a:t>A proportion of 38%  </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1000" b="0" spc="110">
@@ -41183,6 +41159,23 @@
                 </a:r>
               </a:p>
               <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr/>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:solidFill>
@@ -41195,10 +41188,108 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>AESTHETICS : beauty and personal care services</a:t>
+                  <a:t>AESTHETICS : beauty and personal care services, </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>: image and</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>personal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>style</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>consultancy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750">
                     <a:solidFill>
                       <a:schemeClr val="bg1">
                         <a:lumMod val="50000"/>
@@ -41209,6 +41300,15 @@
                   </a:rPr>
                   <a:t> </a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
               <a:p>
                 <a:r>
@@ -41448,8 +41548,43 @@
                     <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
+                  <a:t> , </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>tidying up</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="750">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> </a:t>
                 </a:r>
+                <a:endParaRPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
               <a:p>
                 <a:r>
@@ -41618,7 +41753,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>ARTS &amp;. CULTURE : cultural centers, cultural workshops, free music  concerts in parks and squares, artistic activities, free courses</a:t>
+                  <a:t>ARTS&amp;.CULTURE : cultural centers, cultural workshops, free music  concerts in parks and squares, artistic activities, free courses</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" strike="noStrike" baseline="0">
@@ -41849,7 +41984,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>JOB &amp; BUSINESS: </a:t>
+                  <a:t>JOB&amp;BUSINESS: </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -41906,35 +42041,6 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>HOME SERVICES: tidying up</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
                   <a:t>VOLUNTEER</a:t>
                 </a:r>
                 <a:r>
@@ -41962,119 +42068,6 @@
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
                   <a:t>  </a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>AESTHETICS : image and</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>personal</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>style</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:effectLst/>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>consultancy</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="750">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1">
-                        <a:lumMod val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t> </a:t>
                 </a:r>
               </a:p>
               <a:p>
@@ -42931,45 +42924,49 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>643217</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>58270</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10265" name="AutoShape 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{949460C0-1D1E-D1F0-1A2F-E5BF227CFF4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C2F4D49-5D54-9429-944E-517B2CD2E892}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3750235" y="8142941"/>
-          <a:ext cx="13500100" cy="7289800"/>
+          <a:off x="3746500" y="8140700"/>
+          <a:ext cx="7772400" cy="4203700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
-    </xdr:pic>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -47133,8 +47130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26052D2A-800B-3140-B601-B949F26C3F41}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -47856,11 +47853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I46" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -48879,7 +48876,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update txt and remove a typo in dashboard2
</commit_message>
<xml_diff>
--- a/biwg_dashboards_2.xlsx
+++ b/biwg_dashboards_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcondeixa/repositories/brazilian_immigrant_women_in_germany/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C3B7C8-D96E-1245-B0E4-606997E540E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFFC2C1-84FD-A442-922E-76F36E569812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9980" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="city" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="602">
   <si>
     <t>states</t>
   </si>
@@ -1893,6 +1893,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -4871,7 +4874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{031EC95E-2554-3C4E-8ADE-69A7FE6D50A7}" type="CELLRANGE">
+                    <a:fld id="{F1C3CF73-AEDA-6D48-998B-4AEC8BC06831}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4905,7 +4908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{022F10FB-C2FB-C249-8683-BE958BB2EB5D}" type="CELLRANGE">
+                    <a:fld id="{7ADD66D6-4FE8-5241-A3E8-CCE76AA2BF3F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4939,7 +4942,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA416201-0326-1F40-B061-2BB40FE44863}" type="CELLRANGE">
+                    <a:fld id="{4A06AA65-0619-C14A-A52E-C89EF838BE71}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4973,7 +4976,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDB6B47E-55CB-DC43-ABA2-6FCAB1818937}" type="CELLRANGE">
+                    <a:fld id="{107B7F3A-4A0B-1746-B947-4FBCD5030618}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5007,7 +5010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF20FBF9-0627-5B4C-87BA-1E13C1A18531}" type="CELLRANGE">
+                    <a:fld id="{44AB967D-1E29-674E-86AD-9577998AF327}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5041,7 +5044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8030DB35-D614-C04A-A8B9-18B246B67B30}" type="CELLRANGE">
+                    <a:fld id="{EBF3B052-EF52-1742-8B4A-F6EA03A3D9AE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5075,7 +5078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{592BA5BC-BC48-E649-9BB4-DD34C0459305}" type="CELLRANGE">
+                    <a:fld id="{DE971E56-89B4-FF44-B110-6ABC67819900}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5109,7 +5112,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DE77F5A-8972-DC44-9215-167B6F6F479E}" type="CELLRANGE">
+                    <a:fld id="{E74C69EE-405D-D848-85FD-EDD33C24C2C6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5143,7 +5146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8657AEE2-1DE1-9B46-857F-46BBDBFCF0D2}" type="CELLRANGE">
+                    <a:fld id="{804364F5-0B3E-F548-A525-13D08D8289A2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5177,7 +5180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97FFCD5C-03E5-A547-82F3-E39F8B2338CD}" type="CELLRANGE">
+                    <a:fld id="{2E587897-BA83-4542-870A-D5C3E05ED933}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5211,7 +5214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E0ABB82-503D-8341-AF53-5BF9D7DDF039}" type="CELLRANGE">
+                    <a:fld id="{74B521FB-085A-0C45-A937-7331212220BE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5898,7 +5901,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{11C5CBBD-6F17-D64E-95CC-3CECA3B78A5D}" type="CELLRANGE">
+                    <a:fld id="{FD47B262-6EE3-ED4A-B4AA-EF8FDF954EFD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -5974,7 +5977,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00E70CE0-453E-214E-8C88-2D798A4F4275}" type="CELLRANGE">
+                    <a:fld id="{9610AAB2-F9FF-BC4E-B250-D1129AA7E64F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6008,7 +6011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75731E98-DDFD-D84C-8A4C-221727864200}" type="CELLRANGE">
+                    <a:fld id="{95D98B58-6BBE-384C-8214-938C906834A2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6091,7 +6094,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A0E87DA-BD81-1844-AFD3-37F801EF2A93}" type="CELLRANGE">
+                    <a:fld id="{75D1C617-D531-AF49-8997-DA26D97E5219}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6203,7 +6206,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17BBB576-2A49-C649-8F49-3F1B23FA9D4E}" type="CELLRANGE">
+                    <a:fld id="{F7EC0CE1-79D5-2E44-AA0D-9682DD90D568}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9565,7 +9568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2148BF84-300C-2C4B-8C4E-9084CDC3F954}" type="CELLRANGE">
+                    <a:fld id="{C3EEF80E-D7B3-4344-81AE-13D08512AB82}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9598,7 +9601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D44E3140-B4AE-D344-B2E0-07A192344CE4}" type="CELLRANGE">
+                    <a:fld id="{76383A90-1372-E548-8625-82E3C7B86139}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9632,7 +9635,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA7B32EF-CC54-CD42-B222-2F464845F78E}" type="CELLRANGE">
+                    <a:fld id="{39A87053-B054-4E4B-8DAB-13844E84412D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9666,7 +9669,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F14FD23C-79BB-3B40-A7A1-4DC9D3D50A1A}" type="CELLRANGE">
+                    <a:fld id="{7BA74749-9008-2849-B657-B8D2146373F7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9700,7 +9703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87547110-5426-564F-9DB5-EF3C837402BD}" type="CELLRANGE">
+                    <a:fld id="{7AE07317-C021-AF44-98BD-5A03ECFF8113}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9734,7 +9737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3FF54DD-34F1-2842-B63E-FCCD5DCBB4A1}" type="CELLRANGE">
+                    <a:fld id="{5BC357A3-1FB1-804B-A4F1-A13783A4D562}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10905,7 +10908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{487D8D02-3AAB-D44C-9B11-74B4FBB5E55F}" type="CELLRANGE">
+                    <a:fld id="{2659A59B-57B8-D948-89CA-16A66497D9F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10938,7 +10941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F8A3E1D-C1C1-9345-933A-0782D37C2448}" type="CELLRANGE">
+                    <a:fld id="{FBD9CD6B-F5E8-664B-AC80-746ECFF8B6CC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10972,7 +10975,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2BD1BD26-C614-9D41-8E06-19CBE07FE030}" type="CELLRANGE">
+                    <a:fld id="{93A919AB-F3E0-684A-9484-BA1B367CDFEB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11006,7 +11009,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29FDF726-34F1-8B4D-B61B-2C2EF4399D47}" type="CELLRANGE">
+                    <a:fld id="{BA8AC047-4959-B14D-8CCD-33EC4D79E45F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11040,7 +11043,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53599692-5244-C744-8177-DD20C685EFA8}" type="CELLRANGE">
+                    <a:fld id="{EC6EE0A9-2251-9449-93DF-C6CEA01438E2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11074,7 +11077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B92871D2-AC16-3946-B560-C9A9AC1A33A0}" type="CELLRANGE">
+                    <a:fld id="{4CBF5A37-EA65-B547-A3A0-235424FF4727}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11108,7 +11111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7EB9FF5-668C-4C44-A420-63807B9C56AD}" type="CELLRANGE">
+                    <a:fld id="{85035F60-A005-D44B-B9C7-E7ECD956AC2F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11886,7 +11889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD4692A3-60CE-FA49-8FAE-7D89611CCBEE}" type="CELLRANGE">
+                    <a:fld id="{FE1AB7E3-F9A8-4143-B2B6-89BBD46B9463}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11984,7 +11987,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{601F74A1-0345-0E44-9EB1-B1B70017F969}" type="CELLRANGE">
+                    <a:fld id="{BB7167F8-8A74-AE40-8B45-7CB829990985}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="700"/>
@@ -12060,7 +12063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11AE9168-0AE7-8544-BE62-0A1DD4D731F9}" type="CELLRANGE">
+                    <a:fld id="{DCBF86C2-FA74-544D-B083-A8044CEE6D35}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12094,7 +12097,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E260127E-ECF0-1E48-A44D-E2B9C6A4E74D}" type="CELLRANGE">
+                    <a:fld id="{25C6EAAD-8CE7-3D46-A7E8-1A9DE59288DC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12148,7 +12151,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F947103-80CE-0845-BBA3-A87FE0EF08B3}" type="CELLRANGE">
+                    <a:fld id="{72142382-05EE-8E45-A989-DB76B38F61CB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12202,7 +12205,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEF4B54D-A579-144C-AFCA-1FB7A5B26BE2}" type="CELLRANGE">
+                    <a:fld id="{57C51A4C-A5F1-0840-BCEB-1870F8A76936}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13471,7 +13474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E64423F4-00B8-2B43-A35C-319D23D88C15}" type="CELLRANGE">
+                    <a:fld id="{29000B4B-B518-3F48-8615-05D8C1A13FA3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13505,7 +13508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A725E648-39BE-6C45-A444-1A69A5EA69FD}" type="CELLRANGE">
+                    <a:fld id="{4EC086F8-CFA3-A947-99D4-0F73B99ED200}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13539,7 +13542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11651ACD-BB43-2343-AFE7-0B997427315B}" type="CELLRANGE">
+                    <a:fld id="{6E6E3C97-94C5-C34A-857A-4844D99D2203}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13573,7 +13576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C91F424-6181-E84D-8E8D-0CF0023B5CBE}" type="CELLRANGE">
+                    <a:fld id="{23D57ACA-EEB6-3D41-932C-6DD2941A91BF}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13607,7 +13610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0039C79E-1A3D-D049-915B-89D7BFF8632E}" type="CELLRANGE">
+                    <a:fld id="{D069FB1F-2EC3-4744-AC03-6D54C6EA68E8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -39490,6 +39493,50 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>496047</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>109612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4CEC5AF-32F6-6F21-AA08-BC9877E75931}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8785412"/>
+          <a:ext cx="7772400" cy="4397729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -41188,7 +41235,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>AESTHETICS : beauty and personal care services, </a:t>
+                  <a:t>AESTHETICS : beauty and personal care services,</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike">
@@ -41202,7 +41249,7 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>: image and</a:t>
+                  <a:t> image and</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="750" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -42967,6 +43014,50 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>779929</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>162831</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C2A180-DBB4-0C9B-695E-5549A9E6473E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7888941"/>
+          <a:ext cx="7772400" cy="4196949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -47128,10 +47219,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26052D2A-800B-3140-B601-B949F26C3F41}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -47139,7 +47230,7 @@
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14">
+    <row r="1" spans="1:16" ht="14">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -47153,7 +47244,7 @@
       <c r="K1" s="64"/>
       <c r="L1" s="64"/>
     </row>
-    <row r="2" spans="1:12" ht="14">
+    <row r="2" spans="1:16" ht="14">
       <c r="A2" s="64"/>
       <c r="B2" s="64"/>
       <c r="C2" s="64"/>
@@ -47167,7 +47258,7 @@
       <c r="K2" s="64"/>
       <c r="L2" s="64"/>
     </row>
-    <row r="3" spans="1:12" ht="14">
+    <row r="3" spans="1:16" ht="14">
       <c r="A3" s="64"/>
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
@@ -47181,7 +47272,7 @@
       <c r="K3" s="64"/>
       <c r="L3" s="64"/>
     </row>
-    <row r="4" spans="1:12" ht="14">
+    <row r="4" spans="1:16" ht="14">
       <c r="A4" s="64"/>
       <c r="B4" s="64"/>
       <c r="C4" s="64"/>
@@ -47195,7 +47286,7 @@
       <c r="K4" s="64"/>
       <c r="L4" s="64"/>
     </row>
-    <row r="5" spans="1:12" ht="14">
+    <row r="5" spans="1:16" ht="14">
       <c r="A5" s="64"/>
       <c r="B5" s="64"/>
       <c r="C5" s="64"/>
@@ -47209,7 +47300,7 @@
       <c r="K5" s="64"/>
       <c r="L5" s="64"/>
     </row>
-    <row r="6" spans="1:12" ht="14">
+    <row r="6" spans="1:16" ht="14">
       <c r="A6" s="64"/>
       <c r="B6" s="64"/>
       <c r="C6" s="64"/>
@@ -47223,7 +47314,7 @@
       <c r="K6" s="64"/>
       <c r="L6" s="64"/>
     </row>
-    <row r="7" spans="1:12" ht="14">
+    <row r="7" spans="1:16" ht="14">
       <c r="A7" s="64"/>
       <c r="B7" s="64"/>
       <c r="C7" s="64"/>
@@ -47237,7 +47328,7 @@
       <c r="K7" s="64"/>
       <c r="L7" s="64"/>
     </row>
-    <row r="8" spans="1:12" ht="14">
+    <row r="8" spans="1:16" ht="14">
       <c r="A8" s="64"/>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -47251,7 +47342,7 @@
       <c r="K8" s="64"/>
       <c r="L8" s="64"/>
     </row>
-    <row r="9" spans="1:12" ht="14">
+    <row r="9" spans="1:16" ht="14">
       <c r="A9" s="64"/>
       <c r="B9" s="64"/>
       <c r="C9" s="64"/>
@@ -47265,7 +47356,7 @@
       <c r="K9" s="64"/>
       <c r="L9" s="64"/>
     </row>
-    <row r="10" spans="1:12" ht="14">
+    <row r="10" spans="1:16" ht="14">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -47279,7 +47370,7 @@
       <c r="K10" s="64"/>
       <c r="L10" s="64"/>
     </row>
-    <row r="11" spans="1:12" ht="14">
+    <row r="11" spans="1:16" ht="14">
       <c r="A11" s="64"/>
       <c r="B11" s="64"/>
       <c r="C11" s="64"/>
@@ -47293,7 +47384,7 @@
       <c r="K11" s="64"/>
       <c r="L11" s="64"/>
     </row>
-    <row r="12" spans="1:12" ht="14">
+    <row r="12" spans="1:16" ht="14">
       <c r="A12" s="64"/>
       <c r="B12" s="64"/>
       <c r="C12" s="64"/>
@@ -47307,7 +47398,7 @@
       <c r="K12" s="64"/>
       <c r="L12" s="64"/>
     </row>
-    <row r="13" spans="1:12" ht="14">
+    <row r="13" spans="1:16" ht="14">
       <c r="A13" s="64"/>
       <c r="B13" s="64"/>
       <c r="C13" s="64"/>
@@ -47321,7 +47412,7 @@
       <c r="K13" s="64"/>
       <c r="L13" s="64"/>
     </row>
-    <row r="14" spans="1:12" ht="14">
+    <row r="14" spans="1:16" ht="14">
       <c r="A14" s="64"/>
       <c r="B14" s="64"/>
       <c r="C14" s="64"/>
@@ -47334,8 +47425,11 @@
       <c r="J14" s="64"/>
       <c r="K14" s="64"/>
       <c r="L14" s="64"/>
-    </row>
-    <row r="15" spans="1:12" ht="14">
+      <c r="P14" s="16" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="14">
       <c r="A15" s="64"/>
       <c r="B15" s="64"/>
       <c r="C15" s="64"/>
@@ -47349,7 +47443,7 @@
       <c r="K15" s="64"/>
       <c r="L15" s="64"/>
     </row>
-    <row r="16" spans="1:12" ht="14">
+    <row r="16" spans="1:16" ht="14">
       <c r="A16" s="64"/>
       <c r="B16" s="64"/>
       <c r="C16" s="64"/>
@@ -47856,8 +47950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA0A767-EBAE-2943-ABB2-DBFDA948FD3F}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>